<commit_message>
[FEATURE] Add import / export. Add financial system.
</commit_message>
<xml_diff>
--- a/app/static/ImportVorlage_PfotenRegister.xlsx
+++ b/app/static/ImportVorlage_PfotenRegister.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losc/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losc/PycharmProjects/PfotenRegister/app/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75840CF8-462A-DB49-AF5E-BE016509FA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1057C0D-3683-B240-8C99-70441142F277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68800" yWindow="-7260" windowWidth="68800" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gaeste" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>beduerftigkeit_typ</t>
-  </si>
-  <si>
     <t>dokumente</t>
   </si>
   <si>
@@ -308,6 +305,9 @@
   </si>
   <si>
     <t>02.02.2026</t>
+  </si>
+  <si>
+    <t>beduerftigkeit</t>
   </si>
 </sst>
 </file>
@@ -317,10 +317,10 @@
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="d\.m\.yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="d\.m\.yy;@"/>
-    <numFmt numFmtId="169" formatCode="d\.m;@"/>
-    <numFmt numFmtId="170" formatCode="dd\.mm\.yy;@"/>
+    <numFmt numFmtId="165" formatCode="d\.m\.yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="d\.m\.yy;@"/>
+    <numFmt numFmtId="167" formatCode="d\.m;@"/>
+    <numFmt numFmtId="168" formatCode="dd\.mm\.yy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -409,23 +409,23 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -446,21 +446,19 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <numFmt numFmtId="166" formatCode="d\.m\.yyyy;@"/>
+      <numFmt numFmtId="165" formatCode="d\.m\.yyyy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="dd\.mm\.yy;@"/>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="dd\.mm\.yy;@"/>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="d\.m\.yy;@"/>
+      <numFmt numFmtId="168" formatCode="dd\.mm\.yy;@"/>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -482,12 +480,11 @@
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="dd\.mm\.yy;@"/>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="166" formatCode="d\.m\.yy;@"/>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -495,6 +492,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -538,31 +538,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="GaesteTabelle" displayName="GaesteTabelle" ref="A1:V201" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="GaesteTabelle" displayName="GaesteTabelle" ref="A1:V201" dataDxfId="24">
   <autoFilter ref="A1:V201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="22">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="nummer" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="vorname" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="nachname" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="adresse" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ort" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="plz" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="festnetz" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="mobil" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="email" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="geburtsdatum" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="geschlecht" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="eintritt" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="austritt" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="vertreter_name" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="vertreter_telefon" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="vertreter_email" dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="vertreter_adresse" dataDxfId="11"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="status" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="beduerftigkeit_typ" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="beduerftig_bis" dataDxfId="2"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="dokumente" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="notizen" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="nummer" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="vorname" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="nachname" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="adresse" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ort" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="plz" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="festnetz" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="mobil" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="email" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="geburtsdatum" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="geschlecht" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="eintritt" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="austritt" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="vertreter_name" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="vertreter_telefon" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="vertreter_email" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="vertreter_adresse" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="status" dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="beduerftigkeit" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="beduerftig_bis" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="dokumente" dataDxfId="3"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="notizen" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V201"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1037,16 +1037,16 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
-        <v>68</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="16" x14ac:dyDescent="0.2">
@@ -1054,16 +1054,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F2" s="3">
         <v>4921</v>
@@ -1076,10 +1076,10 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L2" s="7">
         <v>45689</v>
@@ -1090,13 +1090,13 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
@@ -5907,7 +5907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -5919,58 +5919,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" t="s">
-        <v>34</v>
-      </c>
       <c r="R1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -5978,43 +5978,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" t="s">
         <v>85</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" t="s">
         <v>86</v>
       </c>
-      <c r="M2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>87</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -6082,7 +6082,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -6098,7 +6098,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -6114,7 +6114,7 @@
     </row>
     <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -6123,54 +6123,54 @@
     </row>
     <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="11"/>
     </row>
     <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="12">
         <v>1232</v>
@@ -6178,111 +6178,111 @@
     </row>
     <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
         <v>56</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>57</v>
-      </c>
-      <c r="H20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Minor] Add some more fields to animals
</commit_message>
<xml_diff>
--- a/app/static/ImportVorlage_PfotenRegister.xlsx
+++ b/app/static/ImportVorlage_PfotenRegister.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losc/PycharmProjects/PfotenRegister/app/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1057C0D-3683-B240-8C99-70441142F277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FEB21B-2E25-9041-9B34-FB29EB8C8E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gaeste" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>nummer</t>
   </si>
@@ -308,6 +308,12 @@
   </si>
   <si>
     <t>beduerftigkeit</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>steuerbescheid_bis</t>
   </si>
 </sst>
 </file>
@@ -569,14 +575,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TiereTabelle" displayName="TiereTabelle" ref="A1:R212">
-  <autoFilter ref="A1:R212" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TiereTabelle" displayName="TiereTabelle" ref="A1:T212">
+  <autoFilter ref="A1:T212" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="gast_nummer"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="art"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="rasse"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="name"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="geschlecht"/>
+    <tableColumn id="19" xr3:uid="{7485748C-D27F-BB4F-8D20-CF7EE65FB79D}" name="active"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="farbe"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="kastriert"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="identifikation" dataDxfId="1"/>
@@ -587,6 +594,7 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="futter"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="vollversorgung"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="zuletzt_gesehen"/>
+    <tableColumn id="20" xr3:uid="{5DDCBC1E-631E-274A-AFFF-FD66FA9293A0}" name="steuerbescheid_bis"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="tierarzt"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="futtermengeneintrag"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="notizen"/>
@@ -952,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="125" workbookViewId="0">
       <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
@@ -5905,10 +5913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:T212"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5917,7 +5925,7 @@
     <col min="9" max="9" width="25.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -5934,46 +5942,52 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5989,36 +6003,1083 @@
       <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>85</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>61</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>86</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I4" s="10"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H3"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H4"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H5"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H6"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H7"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H10"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H11"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H12"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H13"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H14"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H15"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="H16"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H17"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H18"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H19"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H20"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H21"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H22"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H23"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H24"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H25"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H26"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H27"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H28"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H29"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H30"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H31"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H32"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H33"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H34"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H35"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H36"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H37"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H38"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H39"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H40"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H41"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H42"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H43"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H44"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H45"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H46"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H47"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H48"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H49"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H50"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H51"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H52"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H53"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H54"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H55"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H56"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H57"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H58"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H59"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H60"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H61"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="2"/>
+    </row>
+    <row r="62" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H62"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="2"/>
+    </row>
+    <row r="63" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H63"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="2"/>
+    </row>
+    <row r="64" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H64"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H65"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H66"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H67"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="2"/>
+    </row>
+    <row r="68" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H68"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="2"/>
+    </row>
+    <row r="69" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H69"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="2"/>
+    </row>
+    <row r="70" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H70"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H71"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H72"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="2"/>
+    </row>
+    <row r="73" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H73"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="2"/>
+    </row>
+    <row r="74" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H74"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H75"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H76"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="2"/>
+    </row>
+    <row r="77" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H77"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="2"/>
+    </row>
+    <row r="78" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H78"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="2"/>
+    </row>
+    <row r="79" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H79"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="2"/>
+    </row>
+    <row r="80" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H80"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="2"/>
+    </row>
+    <row r="81" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H81"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="2"/>
+    </row>
+    <row r="82" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H82"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="2"/>
+    </row>
+    <row r="83" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H83"/>
+      <c r="I83" s="9"/>
+      <c r="J83" s="2"/>
+    </row>
+    <row r="84" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H84"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="2"/>
+    </row>
+    <row r="85" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H85"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="2"/>
+    </row>
+    <row r="86" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H86"/>
+      <c r="I86" s="9"/>
+      <c r="J86" s="2"/>
+    </row>
+    <row r="87" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H87"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="2"/>
+    </row>
+    <row r="88" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H88"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="2"/>
+    </row>
+    <row r="89" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H89"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="2"/>
+    </row>
+    <row r="90" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H90"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="2"/>
+    </row>
+    <row r="91" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H91"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="2"/>
+    </row>
+    <row r="92" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H92"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="2"/>
+    </row>
+    <row r="93" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H93"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="2"/>
+    </row>
+    <row r="94" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H94"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H95"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="2"/>
+    </row>
+    <row r="96" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H96"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H97"/>
+      <c r="I97" s="9"/>
+      <c r="J97" s="2"/>
+    </row>
+    <row r="98" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H98"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="2"/>
+    </row>
+    <row r="99" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H99"/>
+      <c r="I99" s="9"/>
+      <c r="J99" s="2"/>
+    </row>
+    <row r="100" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H100"/>
+      <c r="I100" s="9"/>
+      <c r="J100" s="2"/>
+    </row>
+    <row r="101" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H101"/>
+      <c r="I101" s="9"/>
+      <c r="J101" s="2"/>
+    </row>
+    <row r="102" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H102"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="2"/>
+    </row>
+    <row r="103" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H103"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="2"/>
+    </row>
+    <row r="104" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H104"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H105"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="2"/>
+    </row>
+    <row r="106" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H106"/>
+      <c r="I106" s="9"/>
+      <c r="J106" s="2"/>
+    </row>
+    <row r="107" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H107"/>
+      <c r="I107" s="9"/>
+      <c r="J107" s="2"/>
+    </row>
+    <row r="108" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H108"/>
+      <c r="I108" s="9"/>
+      <c r="J108" s="2"/>
+    </row>
+    <row r="109" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H109"/>
+      <c r="I109" s="9"/>
+      <c r="J109" s="2"/>
+    </row>
+    <row r="110" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H110"/>
+      <c r="I110" s="9"/>
+      <c r="J110" s="2"/>
+    </row>
+    <row r="111" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H111"/>
+      <c r="I111" s="9"/>
+      <c r="J111" s="2"/>
+    </row>
+    <row r="112" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H112"/>
+      <c r="I112" s="9"/>
+      <c r="J112" s="2"/>
+    </row>
+    <row r="113" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H113"/>
+      <c r="I113" s="9"/>
+      <c r="J113" s="2"/>
+    </row>
+    <row r="114" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H114"/>
+      <c r="I114" s="9"/>
+      <c r="J114" s="2"/>
+    </row>
+    <row r="115" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H115"/>
+      <c r="I115" s="9"/>
+      <c r="J115" s="2"/>
+    </row>
+    <row r="116" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H116"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="2"/>
+    </row>
+    <row r="117" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H117"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="2"/>
+    </row>
+    <row r="118" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H118"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="2"/>
+    </row>
+    <row r="119" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H119"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="2"/>
+    </row>
+    <row r="120" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H120"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="2"/>
+    </row>
+    <row r="121" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H121"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="2"/>
+    </row>
+    <row r="122" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H122"/>
+      <c r="I122" s="9"/>
+      <c r="J122" s="2"/>
+    </row>
+    <row r="123" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H123"/>
+      <c r="I123" s="9"/>
+      <c r="J123" s="2"/>
+    </row>
+    <row r="124" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H124"/>
+      <c r="I124" s="9"/>
+      <c r="J124" s="2"/>
+    </row>
+    <row r="125" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H125"/>
+      <c r="I125" s="9"/>
+      <c r="J125" s="2"/>
+    </row>
+    <row r="126" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H126"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="2"/>
+    </row>
+    <row r="127" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H127"/>
+      <c r="I127" s="9"/>
+      <c r="J127" s="2"/>
+    </row>
+    <row r="128" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H128"/>
+      <c r="I128" s="9"/>
+      <c r="J128" s="2"/>
+    </row>
+    <row r="129" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H129"/>
+      <c r="I129" s="9"/>
+      <c r="J129" s="2"/>
+    </row>
+    <row r="130" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H130"/>
+      <c r="I130" s="9"/>
+      <c r="J130" s="2"/>
+    </row>
+    <row r="131" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H131"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="2"/>
+    </row>
+    <row r="132" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H132"/>
+      <c r="I132" s="9"/>
+      <c r="J132" s="2"/>
+    </row>
+    <row r="133" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H133"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="2"/>
+    </row>
+    <row r="134" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H134"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="2"/>
+    </row>
+    <row r="135" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H135"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="2"/>
+    </row>
+    <row r="136" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H136"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="2"/>
+    </row>
+    <row r="137" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H137"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="2"/>
+    </row>
+    <row r="138" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H138"/>
+      <c r="I138" s="9"/>
+      <c r="J138" s="2"/>
+    </row>
+    <row r="139" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H139"/>
+      <c r="I139" s="9"/>
+      <c r="J139" s="2"/>
+    </row>
+    <row r="140" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H140"/>
+      <c r="I140" s="9"/>
+      <c r="J140" s="2"/>
+    </row>
+    <row r="141" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H141"/>
+      <c r="I141" s="9"/>
+      <c r="J141" s="2"/>
+    </row>
+    <row r="142" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H142"/>
+      <c r="I142" s="9"/>
+      <c r="J142" s="2"/>
+    </row>
+    <row r="143" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H143"/>
+      <c r="I143" s="9"/>
+      <c r="J143" s="2"/>
+    </row>
+    <row r="144" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H144"/>
+      <c r="I144" s="9"/>
+      <c r="J144" s="2"/>
+    </row>
+    <row r="145" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H145"/>
+      <c r="I145" s="9"/>
+      <c r="J145" s="2"/>
+    </row>
+    <row r="146" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H146"/>
+      <c r="I146" s="9"/>
+      <c r="J146" s="2"/>
+    </row>
+    <row r="147" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H147"/>
+      <c r="I147" s="9"/>
+      <c r="J147" s="2"/>
+    </row>
+    <row r="148" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H148"/>
+      <c r="I148" s="9"/>
+      <c r="J148" s="2"/>
+    </row>
+    <row r="149" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H149"/>
+      <c r="I149" s="9"/>
+      <c r="J149" s="2"/>
+    </row>
+    <row r="150" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H150"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="2"/>
+    </row>
+    <row r="151" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H151"/>
+      <c r="I151" s="9"/>
+      <c r="J151" s="2"/>
+    </row>
+    <row r="152" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H152"/>
+      <c r="I152" s="9"/>
+      <c r="J152" s="2"/>
+    </row>
+    <row r="153" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H153"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="2"/>
+    </row>
+    <row r="154" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H154"/>
+      <c r="I154" s="9"/>
+      <c r="J154" s="2"/>
+    </row>
+    <row r="155" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H155"/>
+      <c r="I155" s="9"/>
+      <c r="J155" s="2"/>
+    </row>
+    <row r="156" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H156"/>
+      <c r="I156" s="9"/>
+      <c r="J156" s="2"/>
+    </row>
+    <row r="157" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H157"/>
+      <c r="I157" s="9"/>
+      <c r="J157" s="2"/>
+    </row>
+    <row r="158" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H158"/>
+      <c r="I158" s="9"/>
+      <c r="J158" s="2"/>
+    </row>
+    <row r="159" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H159"/>
+      <c r="I159" s="9"/>
+      <c r="J159" s="2"/>
+    </row>
+    <row r="160" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H160"/>
+      <c r="I160" s="9"/>
+      <c r="J160" s="2"/>
+    </row>
+    <row r="161" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H161"/>
+      <c r="I161" s="9"/>
+      <c r="J161" s="2"/>
+    </row>
+    <row r="162" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H162"/>
+      <c r="I162" s="9"/>
+      <c r="J162" s="2"/>
+    </row>
+    <row r="163" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H163"/>
+      <c r="I163" s="9"/>
+      <c r="J163" s="2"/>
+    </row>
+    <row r="164" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H164"/>
+      <c r="I164" s="9"/>
+      <c r="J164" s="2"/>
+    </row>
+    <row r="165" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H165"/>
+      <c r="I165" s="9"/>
+      <c r="J165" s="2"/>
+    </row>
+    <row r="166" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H166"/>
+      <c r="I166" s="9"/>
+      <c r="J166" s="2"/>
+    </row>
+    <row r="167" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H167"/>
+      <c r="I167" s="9"/>
+      <c r="J167" s="2"/>
+    </row>
+    <row r="168" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H168"/>
+      <c r="I168" s="9"/>
+      <c r="J168" s="2"/>
+    </row>
+    <row r="169" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H169"/>
+      <c r="I169" s="9"/>
+      <c r="J169" s="2"/>
+    </row>
+    <row r="170" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H170"/>
+      <c r="I170" s="9"/>
+      <c r="J170" s="2"/>
+    </row>
+    <row r="171" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H171"/>
+      <c r="I171" s="9"/>
+      <c r="J171" s="2"/>
+    </row>
+    <row r="172" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H172"/>
+      <c r="I172" s="9"/>
+      <c r="J172" s="2"/>
+    </row>
+    <row r="173" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H173"/>
+      <c r="I173" s="9"/>
+      <c r="J173" s="2"/>
+    </row>
+    <row r="174" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H174"/>
+      <c r="I174" s="9"/>
+      <c r="J174" s="2"/>
+    </row>
+    <row r="175" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H175"/>
+      <c r="I175" s="9"/>
+      <c r="J175" s="2"/>
+    </row>
+    <row r="176" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H176"/>
+      <c r="I176" s="9"/>
+      <c r="J176" s="2"/>
+    </row>
+    <row r="177" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H177"/>
+      <c r="I177" s="9"/>
+      <c r="J177" s="2"/>
+    </row>
+    <row r="178" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H178"/>
+      <c r="I178" s="9"/>
+      <c r="J178" s="2"/>
+    </row>
+    <row r="179" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H179"/>
+      <c r="I179" s="9"/>
+      <c r="J179" s="2"/>
+    </row>
+    <row r="180" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H180"/>
+      <c r="I180" s="9"/>
+      <c r="J180" s="2"/>
+    </row>
+    <row r="181" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H181"/>
+      <c r="I181" s="9"/>
+      <c r="J181" s="2"/>
+    </row>
+    <row r="182" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H182"/>
+      <c r="I182" s="9"/>
+      <c r="J182" s="2"/>
+    </row>
+    <row r="183" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H183"/>
+      <c r="I183" s="9"/>
+      <c r="J183" s="2"/>
+    </row>
+    <row r="184" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H184"/>
+      <c r="I184" s="9"/>
+      <c r="J184" s="2"/>
+    </row>
+    <row r="185" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H185"/>
+      <c r="I185" s="9"/>
+      <c r="J185" s="2"/>
+    </row>
+    <row r="186" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H186"/>
+      <c r="I186" s="9"/>
+      <c r="J186" s="2"/>
+    </row>
+    <row r="187" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H187"/>
+      <c r="I187" s="9"/>
+      <c r="J187" s="2"/>
+    </row>
+    <row r="188" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H188"/>
+      <c r="I188" s="9"/>
+      <c r="J188" s="2"/>
+    </row>
+    <row r="189" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H189"/>
+      <c r="I189" s="9"/>
+      <c r="J189" s="2"/>
+    </row>
+    <row r="190" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H190"/>
+      <c r="I190" s="9"/>
+      <c r="J190" s="2"/>
+    </row>
+    <row r="191" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H191"/>
+      <c r="I191" s="9"/>
+      <c r="J191" s="2"/>
+    </row>
+    <row r="192" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H192"/>
+      <c r="I192" s="9"/>
+      <c r="J192" s="2"/>
+    </row>
+    <row r="193" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H193"/>
+      <c r="I193" s="9"/>
+      <c r="J193" s="2"/>
+    </row>
+    <row r="194" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H194"/>
+      <c r="I194" s="9"/>
+      <c r="J194" s="2"/>
+    </row>
+    <row r="195" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H195"/>
+      <c r="I195" s="9"/>
+      <c r="J195" s="2"/>
+    </row>
+    <row r="196" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H196"/>
+      <c r="I196" s="9"/>
+      <c r="J196" s="2"/>
+    </row>
+    <row r="197" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H197"/>
+      <c r="I197" s="9"/>
+      <c r="J197" s="2"/>
+    </row>
+    <row r="198" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H198"/>
+      <c r="I198" s="9"/>
+      <c r="J198" s="2"/>
+    </row>
+    <row r="199" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H199"/>
+      <c r="I199" s="9"/>
+      <c r="J199" s="2"/>
+    </row>
+    <row r="200" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H200"/>
+      <c r="I200" s="9"/>
+      <c r="J200" s="2"/>
+    </row>
+    <row r="201" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H201"/>
+      <c r="I201" s="9"/>
+      <c r="J201" s="2"/>
+    </row>
+    <row r="202" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H202"/>
+      <c r="I202" s="9"/>
+      <c r="J202" s="2"/>
+    </row>
+    <row r="203" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H203"/>
+      <c r="I203" s="9"/>
+      <c r="J203" s="2"/>
+    </row>
+    <row r="204" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H204"/>
+      <c r="I204" s="9"/>
+      <c r="J204" s="2"/>
+    </row>
+    <row r="205" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H205"/>
+      <c r="I205" s="9"/>
+      <c r="J205" s="2"/>
+    </row>
+    <row r="206" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H206"/>
+      <c r="I206" s="9"/>
+      <c r="J206" s="2"/>
+    </row>
+    <row r="207" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H207"/>
+      <c r="I207" s="9"/>
+      <c r="J207" s="2"/>
+    </row>
+    <row r="208" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H208"/>
+      <c r="I208" s="9"/>
+      <c r="J208" s="2"/>
+    </row>
+    <row r="209" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H209"/>
+      <c r="I209" s="9"/>
+      <c r="J209" s="2"/>
+    </row>
+    <row r="210" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H210"/>
+      <c r="I210" s="9"/>
+      <c r="J210" s="2"/>
+    </row>
+    <row r="211" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H211"/>
+      <c r="I211" s="9"/>
+      <c r="J211" s="2"/>
+    </row>
+    <row r="212" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H212"/>
+      <c r="I212" s="9"/>
+      <c r="J212" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6027,7 +7088,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2727C6B2-EC07-EF4A-9FF1-47B48EE55BD8}">
           <x14:formula1>
             <xm:f>informationen!$D$21:$D$25</xm:f>
@@ -6038,25 +7099,31 @@
           <x14:formula1>
             <xm:f>informationen!$E$21:$E$22</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>E2:E1048576 F3:F212</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6130A95B-51E1-4F46-966B-F7D43861308A}">
           <x14:formula1>
             <xm:f>informationen!$F$21:$F$23</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>G213:G1048576 H2:H212</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9F958B4E-50F0-A34C-936A-1FB1ABB8EEFA}">
           <x14:formula1>
             <xm:f>informationen!$H$21:$H$22</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N1048576</xm:sqref>
+          <xm:sqref>N213:N1048576 O2:O212</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5820EEEF-8704-784C-B73A-B0D4D995E451}">
           <x14:formula1>
             <xm:f>informationen!$G$21:$G$24</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M1048576</xm:sqref>
+          <xm:sqref>M213:M1048576 N2:N212</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CEB9ED6-1EFD-134B-8DF2-5E27B54DA879}">
+          <x14:formula1>
+            <xm:f>informationen!$B$21:$B$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>